<commit_message>
Added shortcuts and shortparse command
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -366,69 +366,58 @@
   <dimension ref="A1:G3"/>
   <sheetData>
     <row r="1" spans="1:7" customFormat="false">
-      <c r="A1" s="0" t="str">
-        <v>Класс</v>
-      </c>
-      <c r="B1" s="0" t="str">
-        <v>Имя</v>
-      </c>
-      <c r="C1" s="0" t="str">
-        <v>Смысл</v>
-      </c>
-      <c r="D1" s="0" t="str">
-        <v>Тип</v>
-      </c>
-      <c r="E1" s="0" t="str">
-        <v>Структура</v>
-      </c>
-      <c r="F1" s="0" t="str">
-        <v>Диапазон</v>
-      </c>
-      <c r="G1" s="0" t="str">
-        <v>Формат</v>
-      </c>
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" spans="1:7" customFormat="false">
       <c r="A2" s="0" t="str">
-        <v>Промежуточные данные</v>
+        <v>Входные данные</v>
       </c>
       <c r="B2" s="0" t="str">
-        <v>a</v>
+        <v>variable</v>
       </c>
       <c r="C2" s="0" t="str">
-        <v>Число для примеру</v>
+        <v>integer</v>
       </c>
       <c r="D2" s="0" t="str">
-        <v>integer, int</v>
+        <v>Простая переменная</v>
       </c>
       <c r="E2" s="0" t="str">
+        <v>0-100</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <v>No format</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <v>does sth</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>Входные данные</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <v>another_variable</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <v>integer</v>
+      </c>
+      <c r="D3" s="0" t="str">
         <v>Простая переменная</v>
       </c>
-      <c r="F2" s="0" t="str">
-        <v>[0 - 100]</v>
-      </c>
-      <c r="G2" s="0" t="str">
-        <v>Число</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" customFormat="false">
-      <c r="A3" s="0" t="str">
-        <v/>
-      </c>
-      <c r="B3" s="0" t="str">
-        <v/>
-      </c>
-      <c r="C3" s="0" t="str">
-        <v>HelloWorld</v>
-      </c>
-      <c r="D3" s="0" t="str">
-        <v/>
-      </c>
       <c r="E3" s="0" t="str">
-        <v/>
+        <v>0-100</v>
       </c>
       <c r="F3" s="0" t="str">
-        <v/>
+        <v>Format</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <v>a really long meaning</v>
       </c>
     </row>
   </sheetData>

</xml_diff>